<commit_message>
working script with tkinter.
</commit_message>
<xml_diff>
--- a/ResultFile.xlsx
+++ b/ResultFile.xlsx
@@ -528,19 +528,19 @@
         </is>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.7748</v>
+        <v>1.77674</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>1.76296</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>13.648212</v>
+        <v>13.6631306</v>
       </c>
       <c r="L2" s="3" t="n">
         <v>13.0106448</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>-0.6375672000000012</v>
+        <v>-0.6524858000000009</v>
       </c>
     </row>
     <row r="3">
@@ -573,19 +573,19 @@
         </is>
       </c>
       <c r="I3" s="3" t="n">
-        <v>1.77657</v>
+        <v>1.7748</v>
       </c>
       <c r="J3" s="3" t="n">
         <v>1.76296</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>21.31884</v>
+        <v>21.2976</v>
       </c>
       <c r="L3" s="3" t="n">
         <v>20.2387808</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>-1.080059200000001</v>
+        <v>-1.058819199999999</v>
       </c>
     </row>
     <row r="4">
@@ -618,24 +618,24 @@
         </is>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1.77657</v>
+        <v>1.7748</v>
       </c>
       <c r="J4" s="3" t="n">
         <v>1.75616</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>14.21256</v>
+        <v>14.1984</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>12.5214208</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>-1.6911392</v>
+        <v>-1.6769792</v>
       </c>
     </row>
     <row r="5">
       <c r="M5" s="3" t="n">
-        <v>-3.408765600000002</v>
+        <v>-3.388284199999999</v>
       </c>
     </row>
   </sheetData>
@@ -754,19 +754,19 @@
         </is>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.75458</v>
+        <v>1.74737</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>1.77787</v>
+        <v>1.77722</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>122.8206</v>
+        <v>122.3159</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>134.5669803</v>
+        <v>134.5177818</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>11.74638030000001</v>
+        <v>12.2018818</v>
       </c>
     </row>
     <row r="3">
@@ -799,24 +799,24 @@
         </is>
       </c>
       <c r="I3" s="3" t="n">
-        <v>1.74006</v>
+        <v>1.72533</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>1.78403</v>
+        <v>1.79979</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>348.012</v>
+        <v>345.066</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>456.8008815</v>
+        <v>460.8362295</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>108.7888815</v>
+        <v>115.7702295</v>
       </c>
     </row>
     <row r="4">
       <c r="M4" s="3" t="n">
-        <v>120.5352618</v>
+        <v>127.9721113</v>
       </c>
     </row>
   </sheetData>
@@ -935,19 +935,19 @@
         </is>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.77674</v>
+        <v>1.7687</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>1.68272</v>
+        <v>1.6781</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>209.7263896</v>
+        <v>208.777348</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>335.8540848</v>
+        <v>334.931979</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>126.1276952</v>
+        <v>126.154631</v>
       </c>
     </row>
     <row r="3">
@@ -980,19 +980,19 @@
         </is>
       </c>
       <c r="I3" s="3" t="n">
-        <v>1.77657</v>
+        <v>1.7748</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>1.68272</v>
+        <v>1.6781</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>51.7337184</v>
+        <v>51.682176</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>77.5229104</v>
+        <v>77.310067</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>25.789192</v>
+        <v>25.62789100000001</v>
       </c>
     </row>
     <row r="4">
@@ -1025,19 +1025,19 @@
         </is>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1.77432</v>
+        <v>1.78094</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>1.68272</v>
+        <v>1.6781</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>6.440781599999999</v>
+        <v>6.4648122</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>7.050596800000001</v>
+        <v>7.031239</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>0.6098152000000017</v>
+        <v>0.5664268000000003</v>
       </c>
     </row>
     <row r="5">
@@ -1073,16 +1073,16 @@
         <v>1.76296</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>1.65552</v>
+        <v>1.6603</v>
       </c>
       <c r="K5" s="3" t="n">
         <v>31.9624648</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>34.5838128</v>
+        <v>34.683667</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>2.621348000000005</v>
+        <v>2.7212022</v>
       </c>
     </row>
     <row r="6">
@@ -1118,16 +1118,16 @@
         <v>1.76296</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>1.68272</v>
+        <v>1.6781</v>
       </c>
       <c r="K6" s="3" t="n">
         <v>88.37718480000001</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>134.7353904</v>
+        <v>134.365467</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>46.35820559999999</v>
+        <v>45.98828219999999</v>
       </c>
     </row>
     <row r="7">
@@ -1163,16 +1163,16 @@
         <v>1.75616</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>1.68272</v>
+        <v>1.6781</v>
       </c>
       <c r="K7" s="3" t="n">
         <v>13.9263488</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>18.173376</v>
+        <v>18.12348</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>4.247027200000002</v>
+        <v>4.197131200000001</v>
       </c>
     </row>
     <row r="8">
@@ -1205,19 +1205,19 @@
         </is>
       </c>
       <c r="I8" s="3" t="n">
-        <v>1.76074</v>
+        <v>1.75112</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>1.61066</v>
+        <v>1.61252</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>176.074</v>
+        <v>175.112</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>295.3467242</v>
+        <v>295.6877924</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>119.2727242</v>
+        <v>120.5757924</v>
       </c>
     </row>
     <row r="9">
@@ -1250,19 +1250,19 @@
         </is>
       </c>
       <c r="I9" s="3" t="n">
-        <v>1.76074</v>
+        <v>1.75112</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>1.66143</v>
+        <v>1.66241</v>
       </c>
       <c r="K9" s="3" t="n">
-        <v>176.074</v>
+        <v>175.112</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>292.577823</v>
+        <v>292.750401</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>116.503823</v>
+        <v>117.638401</v>
       </c>
     </row>
     <row r="10">
@@ -1295,19 +1295,19 @@
         </is>
       </c>
       <c r="I10" s="3" t="n">
-        <v>1.77722</v>
+        <v>1.774</v>
       </c>
       <c r="J10" s="3" t="n">
         <v>1.64938</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>177.722</v>
+        <v>177.4</v>
       </c>
       <c r="L10" s="3" t="n">
         <v>192.2847204</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>14.56272039999999</v>
+        <v>14.88472039999999</v>
       </c>
     </row>
     <row r="11">
@@ -1340,19 +1340,19 @@
         </is>
       </c>
       <c r="I11" s="3" t="n">
-        <v>1.77722</v>
+        <v>1.774</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>1.68272</v>
+        <v>1.6781</v>
       </c>
       <c r="K11" s="3" t="n">
-        <v>170.0088652</v>
+        <v>169.70084</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>251.0954784</v>
+        <v>250.406082</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>81.08661319999999</v>
+        <v>80.705242</v>
       </c>
     </row>
     <row r="12">
@@ -1433,16 +1433,16 @@
         <v>1.78175</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>1.66143</v>
+        <v>1.66241</v>
       </c>
       <c r="K13" s="3" t="n">
         <v>178.175</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>297.894399</v>
+        <v>298.070113</v>
       </c>
       <c r="M13" s="3" t="n">
-        <v>119.719399</v>
+        <v>119.895113</v>
       </c>
     </row>
     <row r="14">
@@ -1475,19 +1475,19 @@
         </is>
       </c>
       <c r="I14" s="3" t="n">
-        <v>1.81246</v>
+        <v>1.81347</v>
       </c>
       <c r="J14" s="3" t="n">
         <v>1.64938</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>181.246</v>
+        <v>181.347</v>
       </c>
       <c r="L14" s="3" t="n">
         <v>238.2364472</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>56.99044720000001</v>
+        <v>56.88944720000003</v>
       </c>
     </row>
     <row r="15">
@@ -1520,19 +1520,19 @@
         </is>
       </c>
       <c r="I15" s="3" t="n">
-        <v>1.81246</v>
+        <v>1.81347</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>1.66143</v>
+        <v>1.66241</v>
       </c>
       <c r="K15" s="3" t="n">
-        <v>181.246</v>
+        <v>181.347</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>300.5859156</v>
+        <v>300.7632172</v>
       </c>
       <c r="M15" s="3" t="n">
-        <v>119.3399156</v>
+        <v>119.4162172</v>
       </c>
     </row>
     <row r="16">
@@ -1565,19 +1565,19 @@
         </is>
       </c>
       <c r="I16" s="3" t="n">
-        <v>1.78403</v>
+        <v>1.79979</v>
       </c>
       <c r="J16" s="3" t="n">
         <v>1.60868</v>
       </c>
       <c r="K16" s="3" t="n">
-        <v>91.9667465</v>
+        <v>92.7791745</v>
       </c>
       <c r="L16" s="3" t="n">
         <v>482.5718264000001</v>
       </c>
       <c r="M16" s="3" t="n">
-        <v>390.6050799000001</v>
+        <v>389.7926519000001</v>
       </c>
     </row>
     <row r="17">
@@ -1610,19 +1610,19 @@
         </is>
       </c>
       <c r="I17" s="3" t="n">
-        <v>1.78403</v>
+        <v>1.79979</v>
       </c>
       <c r="J17" s="3" t="n">
-        <v>1.59477</v>
+        <v>1.60472</v>
       </c>
       <c r="K17" s="3" t="n">
-        <v>358.6792315</v>
+        <v>361.8477795</v>
       </c>
       <c r="L17" s="3" t="n">
-        <v>1345.2841812</v>
+        <v>1353.6776032</v>
       </c>
       <c r="M17" s="3" t="n">
-        <v>986.6049496999999</v>
+        <v>991.8298236999998</v>
       </c>
     </row>
     <row r="18">
@@ -1745,19 +1745,19 @@
         </is>
       </c>
       <c r="I20" s="3" t="n">
-        <v>1.72624</v>
+        <v>1.73852</v>
       </c>
       <c r="J20" s="3" t="n">
-        <v>1.65552</v>
+        <v>1.6603</v>
       </c>
       <c r="K20" s="3" t="n">
-        <v>36.2683024</v>
+        <v>36.5263052</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>50.92379520000001</v>
+        <v>51.07082800000001</v>
       </c>
       <c r="M20" s="3" t="n">
-        <v>14.6554928</v>
+        <v>14.5445228</v>
       </c>
     </row>
     <row r="21">
@@ -1790,19 +1790,19 @@
         </is>
       </c>
       <c r="I21" s="3" t="n">
-        <v>1.72624</v>
+        <v>1.73852</v>
       </c>
       <c r="J21" s="3" t="n">
-        <v>1.66143</v>
+        <v>1.66241</v>
       </c>
       <c r="K21" s="3" t="n">
-        <v>172.624</v>
+        <v>173.852</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>261.4758534</v>
+        <v>261.6300858</v>
       </c>
       <c r="M21" s="3" t="n">
-        <v>88.85185340000001</v>
+        <v>87.77808579999996</v>
       </c>
     </row>
     <row r="22">
@@ -1835,19 +1835,19 @@
         </is>
       </c>
       <c r="I22" s="3" t="n">
-        <v>1.73297</v>
+        <v>1.74628</v>
       </c>
       <c r="J22" s="3" t="n">
-        <v>1.61066</v>
+        <v>1.61252</v>
       </c>
       <c r="K22" s="3" t="n">
-        <v>173.297</v>
+        <v>174.628</v>
       </c>
       <c r="L22" s="3" t="n">
-        <v>282.6386168</v>
+        <v>282.9650096</v>
       </c>
       <c r="M22" s="3" t="n">
-        <v>109.3416168</v>
+        <v>108.3370096</v>
       </c>
     </row>
     <row r="23">
@@ -1880,19 +1880,19 @@
         </is>
       </c>
       <c r="I23" s="3" t="n">
-        <v>1.727</v>
+        <v>1.74254</v>
       </c>
       <c r="J23" s="3" t="n">
-        <v>1.65552</v>
+        <v>1.6603</v>
       </c>
       <c r="K23" s="3" t="n">
-        <v>34.54</v>
+        <v>34.8508</v>
       </c>
       <c r="L23" s="3" t="n">
-        <v>53.32429920000001</v>
+        <v>53.47826300000001</v>
       </c>
       <c r="M23" s="3" t="n">
-        <v>18.78429920000001</v>
+        <v>18.62746300000001</v>
       </c>
     </row>
     <row r="24">
@@ -1925,19 +1925,19 @@
         </is>
       </c>
       <c r="I24" s="3" t="n">
-        <v>1.66241</v>
+        <v>1.66794</v>
       </c>
       <c r="J24" s="3" t="n">
         <v>1.65973</v>
       </c>
       <c r="K24" s="3" t="n">
-        <v>166.2243759</v>
+        <v>166.7773206</v>
       </c>
       <c r="L24" s="3" t="n">
         <v>215.4993432</v>
       </c>
       <c r="M24" s="3" t="n">
-        <v>49.27496730000001</v>
+        <v>48.7220226</v>
       </c>
     </row>
     <row r="25">
@@ -1970,19 +1970,19 @@
         </is>
       </c>
       <c r="I25" s="3" t="n">
-        <v>1.66241</v>
+        <v>1.66794</v>
       </c>
       <c r="J25" s="3" t="n">
-        <v>1.65552</v>
+        <v>1.6603</v>
       </c>
       <c r="K25" s="3" t="n">
-        <v>4.6879962</v>
+        <v>4.7035908</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>7.300843200000001</v>
+        <v>7.321923000000001</v>
       </c>
       <c r="M25" s="3" t="n">
-        <v>2.612847000000001</v>
+        <v>2.618332200000001</v>
       </c>
     </row>
     <row r="26">
@@ -2015,19 +2015,19 @@
         </is>
       </c>
       <c r="I26" s="3" t="n">
-        <v>1.66241</v>
+        <v>1.66171</v>
       </c>
       <c r="J26" s="3" t="n">
-        <v>1.68272</v>
+        <v>1.6781</v>
       </c>
       <c r="K26" s="3" t="n">
-        <v>332.482</v>
+        <v>332.342</v>
       </c>
       <c r="L26" s="3" t="n">
-        <v>455.0411424</v>
+        <v>453.791802</v>
       </c>
       <c r="M26" s="3" t="n">
-        <v>122.5591424</v>
+        <v>121.449802</v>
       </c>
     </row>
     <row r="27">
@@ -2060,24 +2060,24 @@
         </is>
       </c>
       <c r="I27" s="3" t="n">
-        <v>1.67854</v>
+        <v>1.67194</v>
       </c>
       <c r="J27" s="3" t="n">
-        <v>1.70904</v>
+        <v>1.70845</v>
       </c>
       <c r="K27" s="3" t="n">
-        <v>167.854</v>
+        <v>167.194</v>
       </c>
       <c r="L27" s="3" t="n">
-        <v>192.5746272</v>
+        <v>192.508146</v>
       </c>
       <c r="M27" s="3" t="n">
-        <v>24.72062720000002</v>
+        <v>25.31414600000002</v>
       </c>
     </row>
     <row r="28">
       <c r="M28" s="3" t="n">
-        <v>2771.6025395</v>
+        <v>2774.6370952</v>
       </c>
     </row>
   </sheetData>
@@ -2196,19 +2196,19 @@
         </is>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.7086</v>
+        <v>1.70606</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>1.84425</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>72.068748</v>
+        <v>71.9616108</v>
       </c>
       <c r="L2" s="3" t="n">
         <v>79.413405</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>7.344656999999998</v>
+        <v>7.451794199999995</v>
       </c>
     </row>
     <row r="3">
@@ -2286,19 +2286,19 @@
         </is>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1.84896</v>
+        <v>1.82056</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>1.85598</v>
+        <v>1.85845</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>81.539136</v>
+        <v>80.28669600000001</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>63.10332</v>
+        <v>63.1873</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>-18.435816</v>
+        <v>-17.09939600000001</v>
       </c>
     </row>
     <row r="5">
@@ -2334,21 +2334,21 @@
         <v>1.97858</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>1.8226</v>
+        <v>1.81079</v>
       </c>
       <c r="K5" s="3" t="n">
         <v>78.5100544</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>88.286744</v>
+        <v>87.71466759999998</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>9.776689599999997</v>
+        <v>9.204613199999983</v>
       </c>
     </row>
     <row r="6">
       <c r="M6" s="3" t="n">
-        <v>19.7671357</v>
+        <v>20.63861649999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working script with tkinter. Exe file not working yet.
</commit_message>
<xml_diff>
--- a/ResultFile.xlsx
+++ b/ResultFile.xlsx
@@ -528,19 +528,19 @@
         </is>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.77674</v>
+        <v>1.7748</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>1.76296</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>13.6631306</v>
+        <v>13.648212</v>
       </c>
       <c r="L2" s="3" t="n">
         <v>13.0106448</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>-0.6524858000000009</v>
+        <v>-0.6375672000000012</v>
       </c>
     </row>
     <row r="3">
@@ -573,19 +573,19 @@
         </is>
       </c>
       <c r="I3" s="3" t="n">
-        <v>1.7748</v>
+        <v>1.77657</v>
       </c>
       <c r="J3" s="3" t="n">
         <v>1.76296</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>21.2976</v>
+        <v>21.31884</v>
       </c>
       <c r="L3" s="3" t="n">
         <v>20.2387808</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>-1.058819199999999</v>
+        <v>-1.080059200000001</v>
       </c>
     </row>
     <row r="4">
@@ -618,24 +618,24 @@
         </is>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1.7748</v>
+        <v>1.77657</v>
       </c>
       <c r="J4" s="3" t="n">
         <v>1.75616</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>14.1984</v>
+        <v>14.21256</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>12.5214208</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>-1.6769792</v>
+        <v>-1.6911392</v>
       </c>
     </row>
     <row r="5">
       <c r="M5" s="3" t="n">
-        <v>-3.388284199999999</v>
+        <v>-3.408765600000002</v>
       </c>
     </row>
   </sheetData>
@@ -754,19 +754,19 @@
         </is>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.74737</v>
+        <v>1.75458</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>1.77722</v>
+        <v>1.77787</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>122.3159</v>
+        <v>122.8206</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>134.5177818</v>
+        <v>134.5669803</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>12.2018818</v>
+        <v>11.74638030000001</v>
       </c>
     </row>
     <row r="3">
@@ -799,24 +799,24 @@
         </is>
       </c>
       <c r="I3" s="3" t="n">
-        <v>1.72533</v>
+        <v>1.74006</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>1.79979</v>
+        <v>1.78403</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>345.066</v>
+        <v>348.012</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>460.8362295</v>
+        <v>456.8008815</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>115.7702295</v>
+        <v>108.7888815</v>
       </c>
     </row>
     <row r="4">
       <c r="M4" s="3" t="n">
-        <v>127.9721113</v>
+        <v>120.5352618</v>
       </c>
     </row>
   </sheetData>
@@ -935,19 +935,19 @@
         </is>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.7687</v>
+        <v>1.77674</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>1.6781</v>
+        <v>1.68272</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>208.777348</v>
+        <v>209.7263896</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>334.931979</v>
+        <v>335.8540848</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>126.154631</v>
+        <v>126.1276952</v>
       </c>
     </row>
     <row r="3">
@@ -980,19 +980,19 @@
         </is>
       </c>
       <c r="I3" s="3" t="n">
-        <v>1.7748</v>
+        <v>1.77657</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>1.6781</v>
+        <v>1.68272</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>51.682176</v>
+        <v>51.7337184</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>77.310067</v>
+        <v>77.5229104</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>25.62789100000001</v>
+        <v>25.789192</v>
       </c>
     </row>
     <row r="4">
@@ -1025,19 +1025,19 @@
         </is>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1.78094</v>
+        <v>1.77432</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>1.6781</v>
+        <v>1.68272</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>6.4648122</v>
+        <v>6.440781599999999</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>7.031239</v>
+        <v>7.050596800000001</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>0.5664268000000003</v>
+        <v>0.6098152000000017</v>
       </c>
     </row>
     <row r="5">
@@ -1073,16 +1073,16 @@
         <v>1.76296</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>1.6603</v>
+        <v>1.65552</v>
       </c>
       <c r="K5" s="3" t="n">
         <v>31.9624648</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>34.683667</v>
+        <v>34.5838128</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>2.7212022</v>
+        <v>2.621348000000005</v>
       </c>
     </row>
     <row r="6">
@@ -1118,16 +1118,16 @@
         <v>1.76296</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>1.6781</v>
+        <v>1.68272</v>
       </c>
       <c r="K6" s="3" t="n">
         <v>88.37718480000001</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>134.365467</v>
+        <v>134.7353904</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>45.98828219999999</v>
+        <v>46.35820559999999</v>
       </c>
     </row>
     <row r="7">
@@ -1163,16 +1163,16 @@
         <v>1.75616</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>1.6781</v>
+        <v>1.68272</v>
       </c>
       <c r="K7" s="3" t="n">
         <v>13.9263488</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>18.12348</v>
+        <v>18.173376</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>4.197131200000001</v>
+        <v>4.247027200000002</v>
       </c>
     </row>
     <row r="8">
@@ -1205,19 +1205,19 @@
         </is>
       </c>
       <c r="I8" s="3" t="n">
-        <v>1.75112</v>
+        <v>1.76074</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>1.61252</v>
+        <v>1.61066</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>175.112</v>
+        <v>176.074</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>295.6877924</v>
+        <v>295.3467242</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>120.5757924</v>
+        <v>119.2727242</v>
       </c>
     </row>
     <row r="9">
@@ -1250,19 +1250,19 @@
         </is>
       </c>
       <c r="I9" s="3" t="n">
-        <v>1.75112</v>
+        <v>1.76074</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>1.66241</v>
+        <v>1.66143</v>
       </c>
       <c r="K9" s="3" t="n">
-        <v>175.112</v>
+        <v>176.074</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>292.750401</v>
+        <v>292.577823</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>117.638401</v>
+        <v>116.503823</v>
       </c>
     </row>
     <row r="10">
@@ -1295,19 +1295,19 @@
         </is>
       </c>
       <c r="I10" s="3" t="n">
-        <v>1.774</v>
+        <v>1.77722</v>
       </c>
       <c r="J10" s="3" t="n">
         <v>1.64938</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>177.4</v>
+        <v>177.722</v>
       </c>
       <c r="L10" s="3" t="n">
         <v>192.2847204</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>14.88472039999999</v>
+        <v>14.56272039999999</v>
       </c>
     </row>
     <row r="11">
@@ -1340,19 +1340,19 @@
         </is>
       </c>
       <c r="I11" s="3" t="n">
-        <v>1.774</v>
+        <v>1.77722</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>1.6781</v>
+        <v>1.68272</v>
       </c>
       <c r="K11" s="3" t="n">
-        <v>169.70084</v>
+        <v>170.0088652</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>250.406082</v>
+        <v>251.0954784</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>80.705242</v>
+        <v>81.08661319999999</v>
       </c>
     </row>
     <row r="12">
@@ -1433,16 +1433,16 @@
         <v>1.78175</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>1.66241</v>
+        <v>1.66143</v>
       </c>
       <c r="K13" s="3" t="n">
         <v>178.175</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>298.070113</v>
+        <v>297.894399</v>
       </c>
       <c r="M13" s="3" t="n">
-        <v>119.895113</v>
+        <v>119.719399</v>
       </c>
     </row>
     <row r="14">
@@ -1475,19 +1475,19 @@
         </is>
       </c>
       <c r="I14" s="3" t="n">
-        <v>1.81347</v>
+        <v>1.81246</v>
       </c>
       <c r="J14" s="3" t="n">
         <v>1.64938</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>181.347</v>
+        <v>181.246</v>
       </c>
       <c r="L14" s="3" t="n">
         <v>238.2364472</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>56.88944720000003</v>
+        <v>56.99044720000001</v>
       </c>
     </row>
     <row r="15">
@@ -1520,19 +1520,19 @@
         </is>
       </c>
       <c r="I15" s="3" t="n">
-        <v>1.81347</v>
+        <v>1.81246</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>1.66241</v>
+        <v>1.66143</v>
       </c>
       <c r="K15" s="3" t="n">
-        <v>181.347</v>
+        <v>181.246</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>300.7632172</v>
+        <v>300.5859156</v>
       </c>
       <c r="M15" s="3" t="n">
-        <v>119.4162172</v>
+        <v>119.3399156</v>
       </c>
     </row>
     <row r="16">
@@ -1565,19 +1565,19 @@
         </is>
       </c>
       <c r="I16" s="3" t="n">
-        <v>1.79979</v>
+        <v>1.78403</v>
       </c>
       <c r="J16" s="3" t="n">
         <v>1.60868</v>
       </c>
       <c r="K16" s="3" t="n">
-        <v>92.7791745</v>
+        <v>91.9667465</v>
       </c>
       <c r="L16" s="3" t="n">
         <v>482.5718264000001</v>
       </c>
       <c r="M16" s="3" t="n">
-        <v>389.7926519000001</v>
+        <v>390.6050799000001</v>
       </c>
     </row>
     <row r="17">
@@ -1610,19 +1610,19 @@
         </is>
       </c>
       <c r="I17" s="3" t="n">
-        <v>1.79979</v>
+        <v>1.78403</v>
       </c>
       <c r="J17" s="3" t="n">
-        <v>1.60472</v>
+        <v>1.59477</v>
       </c>
       <c r="K17" s="3" t="n">
-        <v>361.8477795</v>
+        <v>358.6792315</v>
       </c>
       <c r="L17" s="3" t="n">
-        <v>1353.6776032</v>
+        <v>1345.2841812</v>
       </c>
       <c r="M17" s="3" t="n">
-        <v>991.8298236999998</v>
+        <v>986.6049496999999</v>
       </c>
     </row>
     <row r="18">
@@ -1745,19 +1745,19 @@
         </is>
       </c>
       <c r="I20" s="3" t="n">
-        <v>1.73852</v>
+        <v>1.72624</v>
       </c>
       <c r="J20" s="3" t="n">
-        <v>1.6603</v>
+        <v>1.65552</v>
       </c>
       <c r="K20" s="3" t="n">
-        <v>36.5263052</v>
+        <v>36.2683024</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>51.07082800000001</v>
+        <v>50.92379520000001</v>
       </c>
       <c r="M20" s="3" t="n">
-        <v>14.5445228</v>
+        <v>14.6554928</v>
       </c>
     </row>
     <row r="21">
@@ -1790,19 +1790,19 @@
         </is>
       </c>
       <c r="I21" s="3" t="n">
-        <v>1.73852</v>
+        <v>1.72624</v>
       </c>
       <c r="J21" s="3" t="n">
-        <v>1.66241</v>
+        <v>1.66143</v>
       </c>
       <c r="K21" s="3" t="n">
-        <v>173.852</v>
+        <v>172.624</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>261.6300858</v>
+        <v>261.4758534</v>
       </c>
       <c r="M21" s="3" t="n">
-        <v>87.77808579999996</v>
+        <v>88.85185340000001</v>
       </c>
     </row>
     <row r="22">
@@ -1835,19 +1835,19 @@
         </is>
       </c>
       <c r="I22" s="3" t="n">
-        <v>1.74628</v>
+        <v>1.73297</v>
       </c>
       <c r="J22" s="3" t="n">
-        <v>1.61252</v>
+        <v>1.61066</v>
       </c>
       <c r="K22" s="3" t="n">
-        <v>174.628</v>
+        <v>173.297</v>
       </c>
       <c r="L22" s="3" t="n">
-        <v>282.9650096</v>
+        <v>282.6386168</v>
       </c>
       <c r="M22" s="3" t="n">
-        <v>108.3370096</v>
+        <v>109.3416168</v>
       </c>
     </row>
     <row r="23">
@@ -1880,19 +1880,19 @@
         </is>
       </c>
       <c r="I23" s="3" t="n">
-        <v>1.74254</v>
+        <v>1.727</v>
       </c>
       <c r="J23" s="3" t="n">
-        <v>1.6603</v>
+        <v>1.65552</v>
       </c>
       <c r="K23" s="3" t="n">
-        <v>34.8508</v>
+        <v>34.54</v>
       </c>
       <c r="L23" s="3" t="n">
-        <v>53.47826300000001</v>
+        <v>53.32429920000001</v>
       </c>
       <c r="M23" s="3" t="n">
-        <v>18.62746300000001</v>
+        <v>18.78429920000001</v>
       </c>
     </row>
     <row r="24">
@@ -1925,19 +1925,19 @@
         </is>
       </c>
       <c r="I24" s="3" t="n">
-        <v>1.66794</v>
+        <v>1.66241</v>
       </c>
       <c r="J24" s="3" t="n">
         <v>1.65973</v>
       </c>
       <c r="K24" s="3" t="n">
-        <v>166.7773206</v>
+        <v>166.2243759</v>
       </c>
       <c r="L24" s="3" t="n">
         <v>215.4993432</v>
       </c>
       <c r="M24" s="3" t="n">
-        <v>48.7220226</v>
+        <v>49.27496730000001</v>
       </c>
     </row>
     <row r="25">
@@ -1970,19 +1970,19 @@
         </is>
       </c>
       <c r="I25" s="3" t="n">
-        <v>1.66794</v>
+        <v>1.66241</v>
       </c>
       <c r="J25" s="3" t="n">
-        <v>1.6603</v>
+        <v>1.65552</v>
       </c>
       <c r="K25" s="3" t="n">
-        <v>4.7035908</v>
+        <v>4.6879962</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>7.321923000000001</v>
+        <v>7.300843200000001</v>
       </c>
       <c r="M25" s="3" t="n">
-        <v>2.618332200000001</v>
+        <v>2.612847000000001</v>
       </c>
     </row>
     <row r="26">
@@ -2015,19 +2015,19 @@
         </is>
       </c>
       <c r="I26" s="3" t="n">
-        <v>1.66171</v>
+        <v>1.66241</v>
       </c>
       <c r="J26" s="3" t="n">
-        <v>1.6781</v>
+        <v>1.68272</v>
       </c>
       <c r="K26" s="3" t="n">
-        <v>332.342</v>
+        <v>332.482</v>
       </c>
       <c r="L26" s="3" t="n">
-        <v>453.791802</v>
+        <v>455.0411424</v>
       </c>
       <c r="M26" s="3" t="n">
-        <v>121.449802</v>
+        <v>122.5591424</v>
       </c>
     </row>
     <row r="27">
@@ -2060,24 +2060,24 @@
         </is>
       </c>
       <c r="I27" s="3" t="n">
-        <v>1.67194</v>
+        <v>1.67854</v>
       </c>
       <c r="J27" s="3" t="n">
-        <v>1.70845</v>
+        <v>1.70904</v>
       </c>
       <c r="K27" s="3" t="n">
-        <v>167.194</v>
+        <v>167.854</v>
       </c>
       <c r="L27" s="3" t="n">
-        <v>192.508146</v>
+        <v>192.5746272</v>
       </c>
       <c r="M27" s="3" t="n">
-        <v>25.31414600000002</v>
+        <v>24.72062720000002</v>
       </c>
     </row>
     <row r="28">
       <c r="M28" s="3" t="n">
-        <v>2774.6370952</v>
+        <v>2771.6025395</v>
       </c>
     </row>
   </sheetData>
@@ -2196,19 +2196,19 @@
         </is>
       </c>
       <c r="I2" s="3" t="n">
-        <v>1.70606</v>
+        <v>1.7086</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>1.84425</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>71.9616108</v>
+        <v>72.068748</v>
       </c>
       <c r="L2" s="3" t="n">
         <v>79.413405</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>7.451794199999995</v>
+        <v>7.344656999999998</v>
       </c>
     </row>
     <row r="3">
@@ -2286,19 +2286,19 @@
         </is>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1.82056</v>
+        <v>1.84896</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>1.85845</v>
+        <v>1.85598</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>80.28669600000001</v>
+        <v>81.539136</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>63.1873</v>
+        <v>63.10332</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>-17.09939600000001</v>
+        <v>-18.435816</v>
       </c>
     </row>
     <row r="5">
@@ -2334,21 +2334,21 @@
         <v>1.97858</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>1.81079</v>
+        <v>1.8226</v>
       </c>
       <c r="K5" s="3" t="n">
         <v>78.5100544</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>87.71466759999998</v>
+        <v>88.286744</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>9.204613199999983</v>
+        <v>9.776689599999997</v>
       </c>
     </row>
     <row r="6">
       <c r="M6" s="3" t="n">
-        <v>20.63861649999998</v>
+        <v>19.7671357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>